<commit_message>
Added more login test cases
</commit_message>
<xml_diff>
--- a/Documentation/MP_Test_Plan.xlsx
+++ b/Documentation/MP_Test_Plan.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Test Scenarios" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
+    <sheet name="Register" sheetId="3" r:id="rId3"/>
+    <sheet name="Logout" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="69">
   <si>
     <t>Project Name</t>
   </si>
@@ -112,9 +114,6 @@
     <t>TC-001</t>
   </si>
   <si>
-    <t>Login to the application with walid username and password</t>
-  </si>
-  <si>
     <t>test_001_login.py</t>
   </si>
   <si>
@@ -131,6 +130,105 @@
   </si>
   <si>
     <t xml:space="preserve">The user should be logged in successfully, the home page should be displayed. </t>
+  </si>
+  <si>
+    <t>TC-002</t>
+  </si>
+  <si>
+    <t>Validate Login with invalid credentials</t>
+  </si>
+  <si>
+    <t>Validate Login to the application with valid username and password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">username: nasko                     password: </t>
+  </si>
+  <si>
+    <t>username: username                           password: Password123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The user should Not be logged in, the Login page should be displayed. </t>
+  </si>
+  <si>
+    <t>Validate Login with invalid username</t>
+  </si>
+  <si>
+    <t>TC-003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ckick on [Sign in ] button on tle right corner.                                            2.Enter invalid username.                                                   3.Enter invalid password                                                         4.Click on [Sign in ] button.   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ckick on [Sign in ] button on tle right corner.                                            2.Enter invalid username.                                                   3.Enter valid password                                                         4.Click on [Sign in ] button.   </t>
+  </si>
+  <si>
+    <t>TC-004</t>
+  </si>
+  <si>
+    <t>TC-005</t>
+  </si>
+  <si>
+    <t>TC-006</t>
+  </si>
+  <si>
+    <t>TC-007</t>
+  </si>
+  <si>
+    <t>TC-008</t>
+  </si>
+  <si>
+    <t>Validate Login with invalid password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ckick on [Sign in ] button on tle right corner.                                            2.Enter valid username.                                                   3.Enter invalid password                                                         4.Click on [Sign in ] button.   </t>
+  </si>
+  <si>
+    <t>username:username                         password: valid_pass</t>
+  </si>
+  <si>
+    <t>username:nasko                         password: Password123</t>
+  </si>
+  <si>
+    <t>Validate Login with valid username and empty password field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ckick on [Sign in ] button on tle right corner.                                            2.Enter valid username.                                                       3.Do not enter password   into the password field                                                      4.Click on [Sign in ] button.   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">username:nasko                         password: </t>
+  </si>
+  <si>
+    <t>username:                         password: Valid_pass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ckick on [Sign in ] button on tle right corner.                                            2.Click on "Reset password" link.   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.The user should Not be logged in,         2.The "Please fill out this field" message should be displayed. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.The user should Not be logged in,        2.The "Please fill out this field" message should be displayed. </t>
+  </si>
+  <si>
+    <t>test_002_registration.py</t>
+  </si>
+  <si>
+    <t>Validate user registration with valid data</t>
+  </si>
+  <si>
+    <t>1. Open the application (http://127.0.0.1:8000/) in any Browser        2. Navigate to the registration page</t>
+  </si>
+  <si>
+    <t>1. Enter new user details into the Mandatory fields (Username, Email, Select Role, Password and Confirm the Password</t>
+  </si>
+  <si>
+    <t>Validate Login with empty username field and valid passwor. Validating the validation message.</t>
+  </si>
+  <si>
+    <t>Validate navigation to the reset password page.  Validating the validation message.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.The user should be navigated to the Reset password page.                                        2.Validation message "Please fill up this field" should be displayed. </t>
   </si>
 </sst>
 </file>
@@ -138,7 +236,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-402]dd\ mmmm\ yyyy\ &quot;г.&quot;;@"/>
+    <numFmt numFmtId="164" formatCode="[$-402]dd\ mmmm\ yyyy\ &quot;г.&quot;;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -322,9 +420,6 @@
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -339,9 +434,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -367,6 +459,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -651,7 +749,7 @@
   <dimension ref="A2:E52"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -663,410 +761,410 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="16">
         <v>45326</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8" t="s">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="8">
-        <v>4</v>
+      <c r="E11" s="6">
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8" t="s">
+      <c r="B12" s="6"/>
+      <c r="C12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="6">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8" t="s">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="6">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="8"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="8"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="8"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="8"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="8"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="8"/>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="8"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
+      <c r="A50" s="6"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="8"/>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
+      <c r="A51" s="6"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="8"/>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="8"/>
+      <c r="A52" s="6"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1077,166 +1175,577 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView topLeftCell="E4" workbookViewId="0">
+      <selection activeCell="E4" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.21875" style="12" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="32.5546875" style="12" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" style="12" customWidth="1"/>
-    <col min="5" max="5" width="43.109375" style="12" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" style="12" customWidth="1"/>
-    <col min="7" max="7" width="31.6640625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="18.44140625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="12"/>
-    <col min="10" max="10" width="12.88671875" style="12" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="12"/>
+    <col min="1" max="1" width="15.21875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="32.5546875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="47.109375" style="10" customWidth="1"/>
+    <col min="6" max="6" width="24.5546875" style="10" customWidth="1"/>
+    <col min="7" max="7" width="36.6640625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="18.44140625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="10"/>
+    <col min="10" max="10" width="12.88671875" style="10" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="81" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F2" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="11"/>
+    </row>
+    <row r="3" spans="1:10" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="11"/>
+    </row>
+    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+    </row>
+    <row r="5" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+    </row>
+    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.21875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="32.5546875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="35.88671875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="47.109375" style="10" customWidth="1"/>
+    <col min="6" max="6" width="24.5546875" style="10" customWidth="1"/>
+    <col min="7" max="7" width="31.6640625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="18.44140625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="10"/>
+    <col min="10" max="10" width="12.88671875" style="10" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="13" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="81" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="14" t="s">
+      <c r="A2" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="12"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+    </row>
+    <row r="3" spans="1:10" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.21875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="32.5546875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="47.109375" style="10" customWidth="1"/>
+    <col min="6" max="6" width="24.5546875" style="10" customWidth="1"/>
+    <col min="7" max="7" width="36.6640625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="18.44140625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="10"/>
+    <col min="10" max="10" width="12.88671875" style="10" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
+      <c r="F1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="81" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+    </row>
+    <row r="3" spans="1:10" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>